<commit_message>
Automation of Valid login test
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B105_Selenium\share\Day26_04_07_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B105_Selenium\share\B105AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CA02FA-F64B-4DBF-BF19-237AE3B75F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6883DAE-3909-43B9-B7FD-38A1A0650FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +38,12 @@
   </si>
   <si>
     <t>akashara</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
   </si>
 </sst>
 </file>
@@ -356,7 +363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -381,4 +388,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD1EA71-C0E6-4185-961D-274A30E7C1A0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Automation of InValid login test
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B105_Selenium\share\B105AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6883DAE-3909-43B9-B7FD-38A1A0650FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2DCE8B-44DC-4AC9-975F-D1746D80F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc1" sheetId="1" r:id="rId1"/>
     <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidLogin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -44,6 +45,15 @@
   </si>
   <si>
     <t>ADMIN</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -394,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD1EA71-C0E6-4185-961D-274A30E7C1A0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -419,4 +429,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88502302-E6BB-48DB-B150-B813FFBA0186}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
For multiple invalid login TC
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B105_Selenium\share\B105AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2DCE8B-44DC-4AC9-975F-D1746D80F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D3B38F-3D2E-4216-988E-6459D6358570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc1" sheetId="1" r:id="rId1"/>
     <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="InvalidLogin" sheetId="3" r:id="rId3"/>
+    <sheet name="MultipleInvalidLogin" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -54,6 +55,9 @@
   </si>
   <si>
     <t>xyz</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -77,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +89,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88502302-E6BB-48DB-B150-B813FFBA0186}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -460,4 +480,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CB4C6B-549D-455E-85F0-D02167D10949}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>